<commit_message>
cat inf slides fixes
</commit_message>
<xml_diff>
--- a/slides/data/recap.xlsx
+++ b/slides/data/recap.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfitzgerald/Library/CloudStorage/GoogleDrive-kfitzgerald@apu.edu/My Drive/MATH_250/APU_MATH_250_public/slides/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9171C063-8224-064D-A43E-6844D711A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D0A7C-E752-864F-B2DA-0BCBAA5DF1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11420" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{0B53D2ED-C862-D04D-9B05-598359DE583D}"/>
+    <workbookView xWindow="7800" yWindow="840" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0B53D2ED-C862-D04D-9B05-598359DE583D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="categorical" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Parameter of Interest</t>
   </si>
@@ -102,6 +103,63 @@
   </si>
   <si>
     <t>lm(), anova()</t>
+  </si>
+  <si>
+    <t>$\hat{p}$</t>
+  </si>
+  <si>
+    <t>$N(0,1)$</t>
+  </si>
+  <si>
+    <t>prop_test()</t>
+  </si>
+  <si>
+    <t>Variable(s) of interest</t>
+  </si>
+  <si>
+    <t>One 2-level categorical variable</t>
+  </si>
+  <si>
+    <t>Two 2-level categorical variables</t>
+  </si>
+  <si>
+    <t>Two 2+ level categorical variables</t>
+  </si>
+  <si>
+    <t>One proportion z-test</t>
+  </si>
+  <si>
+    <t>Hypothesis Test</t>
+  </si>
+  <si>
+    <t>Two proportion z-test</t>
+  </si>
+  <si>
+    <t>$p$</t>
+  </si>
+  <si>
+    <t>$p_1 - p_2$</t>
+  </si>
+  <si>
+    <t>Parameter for CI</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Chi-square test</t>
+  </si>
+  <si>
+    <t>$\hat{p}_1 - \hat{p}_2$</t>
+  </si>
+  <si>
+    <t>$X^2$</t>
+  </si>
+  <si>
+    <t>$\chi^2_{(I-1)(J-1)}$</t>
+  </si>
+  <si>
+    <t>chisq_test() or chisq.test()</t>
   </si>
 </sst>
 </file>
@@ -463,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DC116F-681D-2F4B-BBB2-09ABEAD7A275}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,4 +615,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962D45F-C8A1-8B40-8943-CE42115A34B8}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>